<commit_message>
modify on recieving student credit inputs
</commit_message>
<xml_diff>
--- a/UploadList/UploadStudentList_tid1.xlsx
+++ b/UploadList/UploadStudentList_tid1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\ALLForFYP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/socally/AllFYP/FYPDeploy/UploadList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FCA0BB-05F6-4E70-BAA8-B53802A7EA71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7FA529F-1A5B-754B-B9E2-815B231AD49C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="1776" windowWidth="9816" windowHeight="10584" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>studentname</t>
   </si>
@@ -44,116 +44,84 @@
     <t>topic</t>
   </si>
   <si>
-    <t>Cathy</t>
-  </si>
-  <si>
-    <t>sid33333</t>
-  </si>
-  <si>
-    <t>spw33333</t>
-  </si>
-  <si>
-    <t>how to get abc</t>
-  </si>
-  <si>
-    <t>Dorthy</t>
-  </si>
-  <si>
-    <t>sid44444</t>
-  </si>
-  <si>
-    <t>spw44444</t>
-  </si>
-  <si>
-    <t>where is abc</t>
-  </si>
-  <si>
-    <t>Emily</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Fiona</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gloria</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Helena</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Iris</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Jack</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Kelvin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lemon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sid55555</t>
-  </si>
-  <si>
-    <t>sid66666</t>
-  </si>
-  <si>
-    <t>sid77777</t>
-  </si>
-  <si>
-    <t>sid88888</t>
-  </si>
-  <si>
-    <t>sid99999</t>
-  </si>
-  <si>
-    <t>sid10111</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sid10112</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sid10113</t>
-  </si>
-  <si>
-    <t>spw55555</t>
-  </si>
-  <si>
-    <t>spw66666</t>
-  </si>
-  <si>
-    <t>spw77777</t>
-  </si>
-  <si>
-    <t>spw88888</t>
-  </si>
-  <si>
-    <t>spw99999</t>
-  </si>
-  <si>
-    <t>spw10111</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>spw10112</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>spw10113</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>password</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sid011111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>spw011111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1Cathy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1Dorthy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1Emily</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1Fiona</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1Gloria</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1Helena</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sid012222</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sid013333</t>
+  </si>
+  <si>
+    <t>spw013333</t>
+  </si>
+  <si>
+    <t>spw012222</t>
+  </si>
+  <si>
+    <t>sid014444</t>
+  </si>
+  <si>
+    <t>spw014444</t>
+  </si>
+  <si>
+    <t>sid015555</t>
+  </si>
+  <si>
+    <t>spw015555</t>
+  </si>
+  <si>
+    <t>sid016666</t>
+  </si>
+  <si>
+    <t>spw016666</t>
+  </si>
+  <si>
+    <t>credit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Computational Modeling of Public Health Decision Making for Effective Disease Control</t>
+  </si>
+  <si>
+    <t>Time scheduling of the FYP presentation</t>
+  </si>
+  <si>
+    <t>Nil</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -161,7 +129,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -522,20 +490,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" zoomScale="262" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.5" customWidth="1"/>
     <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="13.77734375" customWidth="1"/>
-    <col min="5" max="7" width="18.109375" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" customWidth="1"/>
+    <col min="5" max="7" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -543,15 +511,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -560,134 +531,98 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C7" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
       <c r="D7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="C8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="19.2" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" t="s">
-        <v>10</v>
-      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="18">
       <c r="F11" s="1"/>
     </row>
   </sheetData>

</xml_diff>